<commit_message>
changes in Rest Assured Main Assignment
</commit_message>
<xml_diff>
--- a/RestAssuredMainAssignment/src/test/resources/CreateUserData.xlsx
+++ b/RestAssuredMainAssignment/src/test/resources/CreateUserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omcv\IdeaProjects\RestAssuredMainAssignment\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F00A51-67DA-4783-B826-0DBD4CBC25F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDDFC1D-AFB7-4DA6-99A1-9D2A8347B7E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A64F3C64-3619-44C7-B64F-01C47DF7AFA9}"/>
   </bookViews>
@@ -48,13 +48,13 @@
     <t>age</t>
   </si>
   <si>
-    <t>kishore@123</t>
-  </si>
-  <si>
-    <t>Anuj Kumar</t>
-  </si>
-  <si>
-    <t>anuj2938@gmail.com</t>
+    <t>virat</t>
+  </si>
+  <si>
+    <t>virat1989@gmail.com</t>
+  </si>
+  <si>
+    <t>virat99k</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -441,13 +441,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D2">
         <v>21</v>
@@ -456,7 +456,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{80742859-EFC1-4DD5-8B71-788AA5329B00}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{E5F494DB-BCF4-4319-9AA1-DAC76272008A}"/>
+    <hyperlink ref="C2" r:id="rId2" display="kishore@123" xr:uid="{E5F494DB-BCF4-4319-9AA1-DAC76272008A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>